<commit_message>
Added dim in file
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Asahi\Sandbox\GitExcelTEst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA643F2-6EA2-4906-883D-12C88BE0FCFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8990F14-6B43-4A2B-B729-D79C1F3D6A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="795" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>